<commit_message>
StockProductos y fixes varios
</commit_message>
<xml_diff>
--- a/excel/StockProductos.xlsx
+++ b/excel/StockProductos.xlsx
@@ -4637,7 +4637,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>191</v>
       </c>
@@ -4645,7 +4645,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>192</v>
       </c>
@@ -4653,15 +4653,18 @@
         <v>23</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>193</v>
       </c>
       <c r="B179" s="1">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="H179" s="1">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>194</v>
       </c>
@@ -4669,7 +4672,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>195</v>
       </c>
@@ -4677,7 +4680,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>196</v>
       </c>
@@ -4685,7 +4688,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>197</v>
       </c>
@@ -4693,7 +4696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>198</v>
       </c>
@@ -4701,7 +4704,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>199</v>
       </c>
@@ -4709,7 +4712,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>200</v>
       </c>
@@ -4717,7 +4720,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>201</v>
       </c>
@@ -4725,7 +4728,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>202</v>
       </c>
@@ -4733,7 +4736,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>203</v>
       </c>
@@ -4741,7 +4744,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
         <v>204</v>
       </c>
@@ -4749,7 +4752,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
         <v>205</v>
       </c>
@@ -4757,7 +4760,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>206</v>
       </c>

</xml_diff>